<commit_message>
:bug: Fix min starting period and check # of months
</commit_message>
<xml_diff>
--- a/data/METEO_PERIOD_2.xlsx
+++ b/data/METEO_PERIOD_2.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1112"/>
+  <dimension ref="A1:G1116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26040,6 +26040,98 @@
         <v>160</v>
       </c>
     </row>
+    <row r="1113">
+      <c r="A1113" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B1113" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1113" t="n">
+        <v>9940</v>
+      </c>
+      <c r="D1113" t="n">
+        <v>9940</v>
+      </c>
+      <c r="E1113" t="n">
+        <v>9900</v>
+      </c>
+      <c r="F1113" t="n">
+        <v>9880</v>
+      </c>
+      <c r="G1113" t="n">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B1114" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1114" t="n">
+        <v>9870</v>
+      </c>
+      <c r="D1114" t="n">
+        <v>9860</v>
+      </c>
+      <c r="E1114" t="n">
+        <v>9810</v>
+      </c>
+      <c r="F1114" t="n">
+        <v>9790</v>
+      </c>
+      <c r="G1114" t="n">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" s="2" t="n">
+        <v>44338</v>
+      </c>
+      <c r="B1115" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1115" t="n">
+        <v>9850</v>
+      </c>
+      <c r="D1115" t="n">
+        <v>9850</v>
+      </c>
+      <c r="E1115" t="n">
+        <v>9850</v>
+      </c>
+      <c r="F1115" t="n">
+        <v>9850</v>
+      </c>
+      <c r="G1115" t="n">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" s="2" t="n">
+        <v>44339</v>
+      </c>
+      <c r="B1116" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1116" t="n">
+        <v>9880</v>
+      </c>
+      <c r="D1116" t="n">
+        <v>9900</v>
+      </c>
+      <c r="E1116" t="n">
+        <v>9900</v>
+      </c>
+      <c r="F1116" t="n">
+        <v>9880</v>
+      </c>
+      <c r="G1116" t="n">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
:bug: Fix alert bug
</commit_message>
<xml_diff>
--- a/data/METEO_PERIOD_2.xlsx
+++ b/data/METEO_PERIOD_2.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1116"/>
+  <dimension ref="A1:G1118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26132,6 +26132,52 @@
         <v>125</v>
       </c>
     </row>
+    <row r="1117">
+      <c r="A1117" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1117" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1117" t="n">
+        <v>9880</v>
+      </c>
+      <c r="D1117" t="n">
+        <v>9880</v>
+      </c>
+      <c r="E1117" t="n">
+        <v>9880</v>
+      </c>
+      <c r="F1117" t="n">
+        <v>9900</v>
+      </c>
+      <c r="G1117" t="n">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1118" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1118" t="n">
+        <v>9940</v>
+      </c>
+      <c r="D1118" t="n">
+        <v>9960</v>
+      </c>
+      <c r="E1118" t="n">
+        <v>9940</v>
+      </c>
+      <c r="F1118" t="n">
+        <v>9920</v>
+      </c>
+      <c r="G1118" t="n">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>